<commit_message>
Added multiple modules Created login window
</commit_message>
<xml_diff>
--- a/accounts.xlsx
+++ b/accounts.xlsx
@@ -460,17 +460,17 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>&lt;function generate_account_number at 0x000002117C962FC0&gt;</t>
+          <t>5392379531</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>connor</t>
+          <t>Connor</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>e23b5fdd175eb04faccc1dd299f5b4d89894919efa2798d225b2e541534fb49a</t>
+          <t>ecd71870d1963316a97e3ac3408c9835ad8cf0f3c1bc703527c30265534f75ae</t>
         </is>
       </c>
       <c r="D2" t="n">
@@ -478,7 +478,7 @@
       </c>
       <c r="E2" t="inlineStr"/>
       <c r="F2" s="1" t="n">
-        <v>46067.55082895506</v>
+        <v>46067.57548154639</v>
       </c>
     </row>
   </sheetData>

</xml_diff>